<commit_message>
hacer titulos mas generales, agregar los datos de posicion al reporte y definir estado de producto disponible por defecto
</commit_message>
<xml_diff>
--- a/core/static/assets/report_templates/report.xlsx
+++ b/core/static/assets/report_templates/report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Projects/Inventario de bodega (BEST)/core/core/static/assets/report_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F02A1D5-E460-2648-A2EA-E837E884706D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF52C749-B72A-AB47-9676-1C70AA2CE9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{D3E0CAD7-EF63-6542-8DAC-0319CB92CDBC}"/>
+    <workbookView xWindow="28980" yWindow="1340" windowWidth="20160" windowHeight="16940" xr2:uid="{D3E0CAD7-EF63-6542-8DAC-0319CB92CDBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t xml:space="preserve">CHOCOLATES BEST DE GUATEMALA </t>
   </si>
@@ -70,12 +70,6 @@
     <t>ALMACEN:</t>
   </si>
   <si>
-    <t>AREA :</t>
-  </si>
-  <si>
-    <t>COS  :</t>
-  </si>
-  <si>
     <t>FECHA:</t>
   </si>
   <si>
@@ -92,6 +86,27 @@
   </si>
   <si>
     <t>DEPTO: BODEGA</t>
+  </si>
+  <si>
+    <t>TIPO DE ALMACENAJE</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>NIVEL</t>
+  </si>
+  <si>
+    <t>POSICION</t>
+  </si>
+  <si>
+    <t>LADO</t>
+  </si>
+  <si>
+    <t>FECHA DE CADUCIDAD</t>
+  </si>
+  <si>
+    <t>RESPONSABLE :</t>
   </si>
 </sst>
 </file>
@@ -158,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -295,38 +310,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,6 +353,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -354,20 +378,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -747,7 +776,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H5" sqref="H5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,72 +784,74 @@
     <col min="1" max="2" width="14.5" customWidth="1"/>
     <col min="3" max="3" width="39.33203125" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="7" t="s">
+      <c r="A2" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="12"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
@@ -830,13 +861,13 @@
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -846,88 +877,94 @@
       <c r="C6" s="22"/>
       <c r="D6" s="22"/>
       <c r="E6" s="23"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="17"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="27" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
     </row>
     <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="D12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="29" t="s">
+      <c r="E12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>17</v>
+      </c>
+      <c r="G12" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:E6"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="H5:J5"/>
@@ -937,6 +974,16 @@
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:J8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
se cambio el formato seleccionar producto y se agregaron cambios en el reporte y se arreglo que salgan solo los del inventario seleccionado
</commit_message>
<xml_diff>
--- a/core/static/assets/report_templates/report.xlsx
+++ b/core/static/assets/report_templates/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Documents/Projects/Inventario de bodega (BEST)/core/core/static/assets/report_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF52C749-B72A-AB47-9676-1C70AA2CE9AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EE4183-9642-3E43-B47F-E8594333171F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28980" yWindow="1340" windowWidth="20160" windowHeight="16940" xr2:uid="{D3E0CAD7-EF63-6542-8DAC-0319CB92CDBC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">CHOCOLATES BEST DE GUATEMALA </t>
   </si>
@@ -73,47 +73,68 @@
     <t>FECHA:</t>
   </si>
   <si>
+    <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>DEPTO: BODEGA</t>
+  </si>
+  <si>
+    <t>TIPO DE ALMACENAJE</t>
+  </si>
+  <si>
+    <t>NIVEL</t>
+  </si>
+  <si>
+    <t>POSICION</t>
+  </si>
+  <si>
+    <t>LADO</t>
+  </si>
+  <si>
+    <t>RESPONSABLE :</t>
+  </si>
+  <si>
+    <t>ALMACEN</t>
+  </si>
+  <si>
+    <t>EMPLEADO</t>
+  </si>
+  <si>
+    <t>FECHA CONTEO</t>
+  </si>
+  <si>
+    <t>BODEGA</t>
+  </si>
+  <si>
+    <t>ARTICULO</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>TIPO DE ARTICULO</t>
+  </si>
+  <si>
+    <t>UDM</t>
+  </si>
+  <si>
+    <t>FECHA VENCE</t>
+  </si>
+  <si>
+    <t>ESTATUS</t>
+  </si>
+  <si>
+    <t>NO.</t>
+  </si>
+  <si>
     <t>SKU</t>
-  </si>
-  <si>
-    <t>MATERIAL</t>
-  </si>
-  <si>
-    <t>DESCRIPCION</t>
-  </si>
-  <si>
-    <t>CANTIDAD</t>
-  </si>
-  <si>
-    <t>DEPTO: BODEGA</t>
-  </si>
-  <si>
-    <t>TIPO DE ALMACENAJE</t>
-  </si>
-  <si>
-    <t>NUMERO</t>
-  </si>
-  <si>
-    <t>NIVEL</t>
-  </si>
-  <si>
-    <t>POSICION</t>
-  </si>
-  <si>
-    <t>LADO</t>
-  </si>
-  <si>
-    <t>FECHA DE CADUCIDAD</t>
-  </si>
-  <si>
-    <t>RESPONSABLE :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -158,6 +179,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -173,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -310,22 +338,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,16 +362,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -378,6 +387,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,12 +417,15 @@
     <xf numFmtId="17" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{A92F4327-C949-B740-8DD6-50459779E483}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -773,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE40FD2-DCB0-0B4A-A743-4A302BC85E70}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:J5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,101 +813,107 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:17" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="12"/>
     </row>
-    <row r="2" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="24"/>
+    <row r="2" spans="1:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="25"/>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="31"/>
     </row>
-    <row r="3" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="5"/>
+      <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="14"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="31"/>
     </row>
-    <row r="5" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="31"/>
     </row>
-    <row r="6" spans="1:10" ht="22" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:17" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20"/>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9" t="s">
@@ -892,75 +922,99 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="33"/>
     </row>
-    <row r="9" spans="1:10" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:17" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="1"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="33"/>
     </row>
-    <row r="12" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="30" t="s">
-        <v>21</v>
+      <c r="O12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q12" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>